<commit_message>
Fixes in report and presentation
</commit_message>
<xml_diff>
--- a/ANOVA.xlsx
+++ b/ANOVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Documents\GitHub\HCI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6763B1-8814-4303-9AD8-F2998E2236BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C60BBD7-6A5F-4984-BD3F-B0A2B4FCDE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15870" xr2:uid="{159F3B5F-E634-40DF-983E-CE70EA40A581}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21270" xr2:uid="{159F3B5F-E634-40DF-983E-CE70EA40A581}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
     <t>Within groups</t>
   </si>
   <si>
-    <t>Su</t>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -221,11 +221,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -574,7 +573,7 @@
   <dimension ref="E4:P71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71:L71"/>
+      <selection activeCell="R64" sqref="R64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,18 +594,18 @@
       </c>
     </row>
     <row r="5" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>20</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>23</v>
       </c>
       <c r="J6" t="s">
@@ -614,95 +613,95 @@
       </c>
     </row>
     <row r="7" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>16</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>14</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>13</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>18</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8">
         <v>15</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8">
         <v>718</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8">
         <v>47.866666666666667</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8">
         <v>21.409523809523815</v>
       </c>
     </row>
     <row r="9" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>30</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>45</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>15</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <v>778</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <v>51.866666666666667</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="1">
         <v>27.123809523809523</v>
       </c>
     </row>
     <row r="10" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>19</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>26</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>27</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>36</v>
       </c>
       <c r="J12" t="s">
@@ -710,10 +709,10 @@
       </c>
     </row>
     <row r="13" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>19</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>27</v>
       </c>
       <c r="J13" t="s">
@@ -739,10 +738,10 @@
       </c>
     </row>
     <row r="14" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>15</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>25</v>
       </c>
       <c r="J14" t="s">
@@ -768,10 +767,10 @@
       </c>
     </row>
     <row r="15" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>12</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>23</v>
       </c>
       <c r="J15" t="s">
@@ -788,18 +787,18 @@
       </c>
     </row>
     <row r="16" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>17</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>24</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>18</v>
       </c>
       <c r="J17" t="s">
@@ -813,70 +812,70 @@
       </c>
     </row>
     <row r="23" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="40" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>1</v>
       </c>
       <c r="J40" t="s">
@@ -884,18 +883,18 @@
       </c>
     </row>
     <row r="41" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E41" s="5">
+      <c r="E41" s="4">
         <v>16</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="4">
         <v>22</v>
       </c>
     </row>
     <row r="42" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E42" s="5">
+      <c r="E42" s="4">
         <v>18</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="4">
         <v>25</v>
       </c>
       <c r="J42" t="s">
@@ -903,95 +902,95 @@
       </c>
     </row>
     <row r="43" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E43" s="5">
+      <c r="E43" s="4">
         <v>23</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="4">
         <v>21</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="K43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L43" s="3" t="s">
+      <c r="L43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M43" s="3" t="s">
+      <c r="M43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N43" s="3" t="s">
+      <c r="N43" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E44" s="5">
+      <c r="E44" s="4">
         <v>17</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="4">
         <v>26</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="J44" t="s">
         <v>0</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44">
         <v>10</v>
       </c>
-      <c r="L44" s="1">
+      <c r="L44">
         <v>188</v>
       </c>
-      <c r="M44" s="1">
+      <c r="M44">
         <v>18.8</v>
       </c>
-      <c r="N44" s="1">
+      <c r="N44">
         <v>6.1777777777777674</v>
       </c>
     </row>
     <row r="45" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E45" s="5">
+      <c r="E45" s="4">
         <v>19</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="4">
         <v>24</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="J45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1">
         <v>10</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L45" s="1">
         <v>236</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="1">
         <v>23.6</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="1">
         <v>6.0444444444444434</v>
       </c>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E46" s="5">
+      <c r="E46" s="4">
         <v>21</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E47" s="5">
+      <c r="E47" s="4">
         <v>16</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="4">
         <v>22</v>
       </c>
     </row>
     <row r="48" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E48" s="5">
+      <c r="E48" s="4">
         <v>22</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="4">
         <v>28</v>
       </c>
       <c r="J48" t="s">
@@ -999,109 +998,97 @@
       </c>
     </row>
     <row r="49" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E49" s="5">
+      <c r="E49" s="4">
         <v>17</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="4">
         <v>25</v>
       </c>
-      <c r="J49" s="3" t="s">
+      <c r="J49" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="K49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L49" s="3" t="s">
+      <c r="L49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M49" s="3" t="s">
+      <c r="M49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N49" s="3" t="s">
+      <c r="N49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O49" s="3" t="s">
+      <c r="O49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P49" s="3" t="s">
+      <c r="P49" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="50" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E50" s="5">
+      <c r="E50" s="4">
         <v>19</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F50" s="4">
         <v>23</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="J50" t="s">
         <v>17</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50">
         <v>115.20000000000003</v>
       </c>
-      <c r="L50" s="1">
+      <c r="L50">
         <v>1</v>
       </c>
-      <c r="M50" s="1">
+      <c r="M50">
         <v>115.20000000000003</v>
       </c>
-      <c r="N50" s="1">
+      <c r="N50">
         <v>18.850909090909099</v>
       </c>
-      <c r="O50" s="1">
+      <c r="O50">
         <v>3.929907022234E-4</v>
       </c>
-      <c r="P50" s="1">
+      <c r="P50">
         <v>4.4138734191705664</v>
       </c>
     </row>
     <row r="51" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="J51" s="1" t="s">
+      <c r="J51" t="s">
         <v>18</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K51">
         <v>109.99999999999999</v>
       </c>
-      <c r="L51" s="1">
+      <c r="L51">
         <v>18</v>
       </c>
-      <c r="M51" s="1">
+      <c r="M51">
         <v>6.1111111111111107</v>
       </c>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-    </row>
-    <row r="52" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
     </row>
     <row r="53" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J53" s="2" t="s">
+      <c r="J53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="1">
         <v>225.20000000000002</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L53" s="1">
         <v>19</v>
       </c>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
     </row>
     <row r="58" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F58" s="6" t="s">
+      <c r="F58" s="5" t="s">
         <v>1</v>
       </c>
       <c r="J58" t="s">
@@ -1109,18 +1096,18 @@
       </c>
     </row>
     <row r="59" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E59" s="5">
+      <c r="E59" s="4">
         <v>46</v>
       </c>
-      <c r="F59" s="5">
+      <c r="F59" s="4">
         <v>53</v>
       </c>
     </row>
     <row r="60" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E60" s="5">
+      <c r="E60" s="4">
         <v>48</v>
       </c>
-      <c r="F60" s="5">
+      <c r="F60" s="4">
         <v>56</v>
       </c>
       <c r="J60" t="s">
@@ -1128,95 +1115,95 @@
       </c>
     </row>
     <row r="61" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E61" s="5">
+      <c r="E61" s="4">
         <v>54</v>
       </c>
-      <c r="F61" s="5">
+      <c r="F61" s="4">
         <v>51</v>
       </c>
-      <c r="J61" s="3" t="s">
+      <c r="J61" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="K61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L61" s="3" t="s">
+      <c r="L61" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M61" s="3" t="s">
+      <c r="M61" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N61" s="3" t="s">
+      <c r="N61" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E62" s="5">
+      <c r="E62" s="4">
         <v>47</v>
       </c>
-      <c r="F62" s="5">
+      <c r="F62" s="4">
         <v>58</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="J62" t="s">
         <v>0</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K62">
         <v>8</v>
       </c>
-      <c r="L62" s="1">
+      <c r="L62">
         <v>396</v>
       </c>
-      <c r="M62" s="1">
+      <c r="M62">
         <v>49.5</v>
       </c>
-      <c r="N62" s="1">
+      <c r="N62">
         <v>10.285714285714286</v>
       </c>
     </row>
     <row r="63" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E63" s="5">
+      <c r="E63" s="4">
         <v>50</v>
       </c>
-      <c r="F63" s="5">
+      <c r="F63" s="4">
         <v>55</v>
       </c>
-      <c r="J63" s="2" t="s">
+      <c r="J63" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="1">
         <v>8</v>
       </c>
-      <c r="L63" s="2">
+      <c r="L63" s="1">
         <v>436</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="1">
         <v>54.5</v>
       </c>
-      <c r="N63" s="2">
+      <c r="N63" s="1">
         <v>12.857142857142858</v>
       </c>
     </row>
     <row r="64" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E64" s="5">
+      <c r="E64" s="4">
         <v>52</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F64" s="4">
         <v>49</v>
       </c>
     </row>
     <row r="65" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E65" s="5">
+      <c r="E65" s="4">
         <v>46</v>
       </c>
-      <c r="F65" s="5">
+      <c r="F65" s="4">
         <v>54</v>
       </c>
     </row>
     <row r="66" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E66" s="5">
+      <c r="E66" s="4">
         <v>53</v>
       </c>
-      <c r="F66" s="5">
+      <c r="F66" s="4">
         <v>60</v>
       </c>
       <c r="J66" t="s">
@@ -1224,103 +1211,91 @@
       </c>
     </row>
     <row r="67" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E67" s="5">
+      <c r="E67" s="4">
         <v>47</v>
       </c>
-      <c r="F67" s="5">
+      <c r="F67" s="4">
         <v>56</v>
       </c>
-      <c r="J67" s="3" t="s">
+      <c r="J67" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K67" s="3" t="s">
+      <c r="K67" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L67" s="3" t="s">
+      <c r="L67" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M67" s="3" t="s">
+      <c r="M67" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N67" s="3" t="s">
+      <c r="N67" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O67" s="3" t="s">
+      <c r="O67" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P67" s="3" t="s">
+      <c r="P67" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="68" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E68" s="5">
+      <c r="E68" s="4">
         <v>49</v>
       </c>
-      <c r="F68" s="5">
+      <c r="F68" s="4">
         <v>52</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="J68" t="s">
         <v>35</v>
       </c>
-      <c r="K68" s="1">
+      <c r="K68">
         <v>100</v>
       </c>
-      <c r="L68" s="1">
+      <c r="L68">
         <v>1</v>
       </c>
-      <c r="M68" s="1">
+      <c r="M68">
         <v>100</v>
       </c>
-      <c r="N68" s="1">
+      <c r="N68">
         <v>8.6419753086419764</v>
       </c>
-      <c r="O68" s="1">
+      <c r="O68">
         <v>1.0762558178722806E-2</v>
       </c>
-      <c r="P68" s="1">
+      <c r="P68">
         <v>4.6001099366694227</v>
       </c>
     </row>
     <row r="69" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="J69" s="1" t="s">
+      <c r="J69" t="s">
         <v>36</v>
       </c>
-      <c r="K69" s="1">
+      <c r="K69">
         <v>162</v>
       </c>
-      <c r="L69" s="1">
+      <c r="L69">
         <v>14</v>
       </c>
-      <c r="M69" s="1">
+      <c r="M69">
         <v>11.571428571428571</v>
       </c>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-    </row>
-    <row r="70" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
     </row>
     <row r="71" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J71" s="2" t="s">
+      <c r="J71" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K71" s="2">
+      <c r="K71" s="1">
         <v>262</v>
       </c>
-      <c r="L71" s="2">
+      <c r="L71" s="1">
         <v>15</v>
       </c>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="2"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>